<commit_message>
Updated for new functionality. Improved NMR data processing, overhauled MATLAB and dFBA code.
</commit_message>
<xml_diff>
--- a/data/coeffs.xlsx
+++ b/data/coeffs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apavao/repos/nmr-cdiff/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F2BF8194-852C-C84D-95B9-77A08023C08E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D053A4F7-54A7-DF4D-BD32-9874612A1AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27640" windowHeight="16940" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cf" sheetId="1" r:id="rId1"/>
@@ -50,9 +50,6 @@
     <t>c</t>
   </si>
   <si>
-    <t>glc</t>
-  </si>
-  <si>
     <t>eto</t>
   </si>
   <si>
@@ -85,11 +82,14 @@
   <si>
     <t>isocap</t>
   </si>
+  <si>
+    <t>glc</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -923,11 +923,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:E13"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -951,7 +951,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B2">
         <v>26.975441715296807</v>
@@ -968,7 +968,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>6.7687705930713369</v>
@@ -985,7 +985,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>12.776293567874589</v>
@@ -1002,7 +1002,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>14.00417375517492</v>
@@ -1019,7 +1019,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>3.9928419306383338</v>
@@ -1036,7 +1036,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>6.1815410660444092</v>
@@ -1053,7 +1053,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>3.2128258949005866</v>
@@ -1070,10 +1070,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9">
-        <v>3.003442854276634</v>
+        <v>4.0045904723688448</v>
       </c>
       <c r="C9">
         <v>-0.45735078498372128</v>
@@ -1082,15 +1082,15 @@
         <v>11.216599095619713</v>
       </c>
       <c r="E9">
-        <v>2.2165571457233662</v>
+        <v>2.9554095276311547</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10">
-        <v>2.9830309140000835</v>
+        <v>3.9773745520001111</v>
       </c>
       <c r="C10">
         <v>0.64123545400628634</v>
@@ -1104,33 +1104,33 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11">
-        <v>7.1994969586731941</v>
+        <v>7.63</v>
       </c>
       <c r="C11">
-        <v>-0.59125046661610825</v>
+        <v>-0.53374918531371707</v>
       </c>
       <c r="D11">
-        <v>8.088776625630393</v>
+        <v>8.2882989136034873</v>
       </c>
       <c r="E11">
-        <v>0.43050304132680584</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12">
-        <v>2.3051268536254064</v>
+        <v>2.1853930592703086</v>
       </c>
       <c r="C12">
-        <v>0.73137425286074775</v>
+        <v>0.71615649391571201</v>
       </c>
       <c r="D12">
-        <v>4.6555268140678496</v>
+        <v>4.6677561747542491</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -1138,16 +1138,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13">
-        <v>5.1643597316370462</v>
+        <v>5.1832807094315205</v>
       </c>
       <c r="C13">
-        <v>0.92644099556075366</v>
+        <v>0.89761277885073454</v>
       </c>
       <c r="D13">
-        <v>9.8564212495014019</v>
+        <v>9.8755992348235733</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -1159,11 +1159,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1187,33 +1187,33 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B2">
-        <v>27.558432267967394</v>
+        <v>26.530363328679737</v>
       </c>
       <c r="C2">
-        <v>-0.15346873044376122</v>
+        <v>-0.10748393003633491</v>
       </c>
       <c r="D2">
-        <v>14.431962493978203</v>
+        <v>18.430296587256777</v>
       </c>
       <c r="E2">
-        <v>-5.8432267967392405E-2</v>
+        <v>0.96963667132026454</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3">
-        <v>7.271815100314253</v>
+        <v>6.3698442557035593</v>
       </c>
       <c r="C3">
-        <v>0.15356365406767719</v>
+        <v>0.2637715953076068</v>
       </c>
       <c r="D3">
-        <v>22.097789302611794</v>
+        <v>25.047260317022705</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -1221,7 +1221,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>12.186993683681795</v>
@@ -1238,7 +1238,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>13.31039047557311</v>
@@ -1255,7 +1255,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>3.2922075516615887</v>
@@ -1272,7 +1272,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>5.7343715486349742</v>
@@ -1289,7 +1289,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>2.5675857103219473</v>
@@ -1306,10 +1306,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9">
-        <v>2.9601229689496948</v>
+        <v>3.9468306252662599</v>
       </c>
       <c r="C9">
         <v>-0.52514868823439298</v>
@@ -1318,15 +1318,15 @@
         <v>10.902383734719804</v>
       </c>
       <c r="E9">
-        <v>2.2598770310503054</v>
+        <v>3.0131693747337405</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10">
-        <v>3.0121901109812956</v>
+        <v>4.0162534813083939</v>
       </c>
       <c r="C10">
         <v>0.49791111319785514</v>
@@ -1340,33 +1340,33 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11">
-        <v>7.3136138169130964</v>
+        <v>7.63</v>
       </c>
       <c r="C11">
-        <v>-0.68874761150469044</v>
+        <v>-0.64410115587848005</v>
       </c>
       <c r="D11">
-        <v>7.7674902613643972</v>
+        <v>7.8422898637383822</v>
       </c>
       <c r="E11">
-        <v>0.31638618308690397</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12">
-        <v>2.2943282405033387</v>
+        <v>2.1369391201172645</v>
       </c>
       <c r="C12">
-        <v>0.36534079197300962</v>
+        <v>0.34521769080321613</v>
       </c>
       <c r="D12">
-        <v>3.8729283966219157</v>
+        <v>3.8404564183549121</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -1374,16 +1374,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13">
-        <v>5.2850407242480788</v>
+        <v>5.2252688170940749</v>
       </c>
       <c r="C13">
-        <v>0.71735580395754028</v>
+        <v>0.70172750036117071</v>
       </c>
       <c r="D13">
-        <v>9.5770078119557063</v>
+        <v>9.596959097846355</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -1395,11 +1395,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1423,33 +1423,33 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B2">
-        <v>26.530363328679737</v>
+        <v>27.558432267967394</v>
       </c>
       <c r="C2">
-        <v>-0.10748393003633491</v>
+        <v>-0.15346873044376122</v>
       </c>
       <c r="D2">
-        <v>18.430296587256777</v>
+        <v>14.431962493978203</v>
       </c>
       <c r="E2">
-        <v>0.96963667132026454</v>
+        <v>-5.8432267967392405E-2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3">
-        <v>6.3698442557035593</v>
+        <v>7.271815100314253</v>
       </c>
       <c r="C3">
-        <v>0.2637715953076068</v>
+        <v>0.15356365406767719</v>
       </c>
       <c r="D3">
-        <v>25.047260317022705</v>
+        <v>22.097789302611794</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -1457,7 +1457,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>13.368155238456019</v>
@@ -1474,7 +1474,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>14.701993655958612</v>
@@ -1491,7 +1491,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>4.70753862803135</v>
@@ -1508,7 +1508,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>6.6341111105320145</v>
@@ -1525,7 +1525,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>3.8476799062968516</v>
@@ -1542,10 +1542,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9">
-        <v>3.0437698437942386</v>
+        <v>4.0583597917256515</v>
       </c>
       <c r="C9">
         <v>-0.38955288173304953</v>
@@ -1554,15 +1554,15 @@
         <v>11.530814456519623</v>
       </c>
       <c r="E9">
-        <v>2.1762301562057611</v>
+        <v>2.901640208274348</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10">
-        <v>2.9558862754090884</v>
+        <v>3.9411817005454517</v>
       </c>
       <c r="C10">
         <v>0.7845597948147176</v>
@@ -1576,33 +1576,33 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11">
-        <v>7.0947499916516907</v>
+        <v>7.63</v>
       </c>
       <c r="C11">
-        <v>-0.49375332172752612</v>
+        <v>-0.42339721474895409</v>
       </c>
       <c r="D11">
-        <v>8.4100629898963888</v>
+        <v>8.7343079634685914</v>
       </c>
       <c r="E11">
-        <v>0.53525000834830949</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12">
-        <v>2.3150388157142792</v>
+        <v>2.2312095499167066</v>
       </c>
       <c r="C12">
-        <v>1.0974077137484859</v>
+        <v>1.087095297028208</v>
       </c>
       <c r="D12">
-        <v>5.4381252315137836</v>
+        <v>5.495055931153586</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -1610,16 +1610,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13">
-        <v>5.0535875972817896</v>
+        <v>5.1435781016434285</v>
       </c>
       <c r="C13">
-        <v>1.135526187163967</v>
+        <v>1.0934980573402984</v>
       </c>
       <c r="D13">
-        <v>10.135834687047097</v>
+        <v>10.154239371800792</v>
       </c>
       <c r="E13">
         <v>0</v>

</xml_diff>